<commit_message>
minor speed bump from dma rectangel mod to hagl
</commit_message>
<xml_diff>
--- a/driver/display/hagl_hal/perf.xlsx
+++ b/driver/display/hagl_hal/perf.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Default VSync</t>
   </si>
@@ -36,7 +36,10 @@
     <t xml:space="preserve">DMA No Malloc</t>
   </si>
   <si>
-    <t xml:space="preserve">No Malloc Direct HLine</t>
+    <t xml:space="preserve">Static Direct HLine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectangle DMA</t>
   </si>
   <si>
     <t xml:space="preserve">HAGL TDMA</t>
@@ -134,7 +137,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
@@ -659,8 +663,9 @@
     <col min="5" max="5" width="10.54296875"/>
     <col bestFit="1" min="6" max="6" width="16.48046875"/>
     <col bestFit="1" customWidth="1" min="8" max="8" width="14.3125"/>
-    <col bestFit="1" min="9" max="9" width="20.25390625"/>
-    <col bestFit="1" min="10" max="10" width="11.34375"/>
+    <col bestFit="1" min="9" max="9" width="15.890625"/>
+    <col bestFit="1" min="10" max="10" width="13.61328125"/>
+    <col bestFit="1" min="11" max="11" width="11.34375"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -688,13 +693,16 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>63</v>
@@ -708,7 +716,7 @@
       <c r="E2">
         <v>399</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>335</v>
       </c>
       <c r="G2">
@@ -719,11 +727,14 @@
       </c>
       <c r="I2">
         <v>3505</v>
+      </c>
+      <c r="J2">
+        <v>4020</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>358167</v>
@@ -737,7 +748,7 @@
       <c r="E3">
         <v>427404</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>358612</v>
       </c>
       <c r="G3">
@@ -750,16 +761,15 @@
         <v>427700</v>
       </c>
       <c r="J3">
+        <v>427722</v>
+      </c>
+      <c r="K3">
         <v>365326</v>
-      </c>
-      <c r="K3">
-        <f>I3/J3</f>
-        <v>1.1707351789908191</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>14427</v>
@@ -773,7 +783,7 @@
       <c r="E4">
         <v>17167</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>14336</v>
       </c>
       <c r="G4">
@@ -786,16 +796,15 @@
         <v>17238</v>
       </c>
       <c r="J4">
+        <v>17226</v>
+      </c>
+      <c r="K4">
         <v>17794</v>
-      </c>
-      <c r="K4">
-        <f>I4/J4</f>
-        <v>0.96875351241991681</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>25514</v>
@@ -809,7 +818,7 @@
       <c r="E5">
         <v>75765</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>63697</v>
       </c>
       <c r="G5">
@@ -822,16 +831,15 @@
         <v>103181</v>
       </c>
       <c r="J5">
+        <v>103071</v>
+      </c>
+      <c r="K5">
         <v>82509</v>
-      </c>
-      <c r="K5">
-        <f>I5/J5</f>
-        <v>1.2505423650753251</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>31491</v>
@@ -845,7 +853,7 @@
       <c r="E6">
         <v>142198</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="3">
         <v>119233</v>
       </c>
       <c r="G6">
@@ -858,16 +866,15 @@
         <v>285072</v>
       </c>
       <c r="J6">
+        <v>285209</v>
+      </c>
+      <c r="K6">
         <v>82497</v>
-      </c>
-      <c r="K6">
-        <f>I6/J6</f>
-        <v>3.4555438379577441</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>15214</v>
@@ -881,7 +888,7 @@
       <c r="E7">
         <v>18142</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="3">
         <v>15209</v>
       </c>
       <c r="G7">
@@ -894,16 +901,15 @@
         <v>18215</v>
       </c>
       <c r="J7">
+        <v>18171</v>
+      </c>
+      <c r="K7">
         <v>15371</v>
-      </c>
-      <c r="K7">
-        <f>I7/J7</f>
-        <v>1.1850237460152235</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>838</v>
@@ -917,7 +923,7 @@
       <c r="E8">
         <v>3568</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="3">
         <v>2973</v>
       </c>
       <c r="G8">
@@ -930,16 +936,15 @@
         <v>16126</v>
       </c>
       <c r="J8">
+        <v>16139</v>
+      </c>
+      <c r="K8">
         <v>9744</v>
-      </c>
-      <c r="K8">
-        <f>I8/J8</f>
-        <v>1.6549671592775042</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>7873</v>
@@ -953,7 +958,7 @@
       <c r="E9">
         <v>9396</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="3">
         <v>7892</v>
       </c>
       <c r="G9">
@@ -966,16 +971,15 @@
         <v>9402</v>
       </c>
       <c r="J9">
+        <v>9410</v>
+      </c>
+      <c r="K9">
         <v>8563</v>
-      </c>
-      <c r="K9">
-        <f>I9/J9</f>
-        <v>1.097979680018685</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>307</v>
@@ -989,7 +993,7 @@
       <c r="E10">
         <v>1502</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="3">
         <v>1358</v>
       </c>
       <c r="G10">
@@ -1002,16 +1006,15 @@
         <v>7835</v>
       </c>
       <c r="J10">
+        <v>7833</v>
+      </c>
+      <c r="K10">
         <v>4167</v>
-      </c>
-      <c r="K10">
-        <f>I10/J10</f>
-        <v>1.8802495800335972</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>4881</v>
@@ -1025,7 +1028,7 @@
       <c r="E11">
         <v>5883</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="3">
         <v>4917</v>
       </c>
       <c r="G11">
@@ -1038,16 +1041,15 @@
         <v>5841</v>
       </c>
       <c r="J11">
+        <v>5844</v>
+      </c>
+      <c r="K11">
         <v>6080</v>
-      </c>
-      <c r="K11">
-        <f>I11/J11</f>
-        <v>0.96069078947368425</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>252</v>
@@ -1061,7 +1063,7 @@
       <c r="E12">
         <v>496</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="3">
         <v>417</v>
       </c>
       <c r="G12">
@@ -1074,16 +1076,15 @@
         <v>628</v>
       </c>
       <c r="J12">
+        <v>625</v>
+      </c>
+      <c r="K12">
         <v>806</v>
-      </c>
-      <c r="K12">
-        <f>I12/J12</f>
-        <v>0.77915632754342434</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>5692</v>
@@ -1097,7 +1098,7 @@
       <c r="E13">
         <v>22063</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="3">
         <v>18620</v>
       </c>
       <c r="G13">
@@ -1110,16 +1111,15 @@
         <v>34738</v>
       </c>
       <c r="J13">
+        <v>34755</v>
+      </c>
+      <c r="K13">
         <v>25244</v>
-      </c>
-      <c r="K13">
-        <f>I13/J13</f>
-        <v>1.3760893677705592</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>405</v>
@@ -1133,7 +1133,7 @@
       <c r="E14">
         <v>2788</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="3">
         <v>2326</v>
       </c>
       <c r="G14">
@@ -1146,16 +1146,15 @@
         <v>19863</v>
       </c>
       <c r="J14">
+        <v>26099</v>
+      </c>
+      <c r="K14">
         <v>10712</v>
-      </c>
-      <c r="K14">
-        <f>I14/J14</f>
-        <v>1.8542755787901419</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>5503</v>
@@ -1169,7 +1168,7 @@
       <c r="E15">
         <v>16840</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="3">
         <v>14121</v>
       </c>
       <c r="G15">
@@ -1182,16 +1181,15 @@
         <v>24369</v>
       </c>
       <c r="J15">
+        <v>24417</v>
+      </c>
+      <c r="K15">
         <v>19288</v>
-      </c>
-      <c r="K15">
-        <f>I15/J15</f>
-        <v>1.2634280381584404</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>427</v>
@@ -1205,7 +1203,7 @@
       <c r="E16">
         <v>2555</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="3">
         <v>2138</v>
       </c>
       <c r="G16">
@@ -1218,16 +1216,15 @@
         <v>16860</v>
       </c>
       <c r="J16">
+        <v>21285</v>
+      </c>
+      <c r="K16">
         <v>9347</v>
-      </c>
-      <c r="K16">
-        <f>I16/J16</f>
-        <v>1.8037873114368246</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>2967</v>
@@ -1241,7 +1238,7 @@
       <c r="E17">
         <v>3536</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="3">
         <v>2964</v>
       </c>
       <c r="G17">
@@ -1254,16 +1251,15 @@
         <v>3535</v>
       </c>
       <c r="J17">
+        <v>3534</v>
+      </c>
+      <c r="K17">
         <v>3678</v>
-      </c>
-      <c r="K17">
-        <f>I17/J17</f>
-        <v>0.96112017400761285</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>144</v>
@@ -1277,7 +1273,7 @@
       <c r="E18">
         <v>266</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="3">
         <v>227</v>
       </c>
       <c r="G18">
@@ -1290,16 +1286,15 @@
         <v>335</v>
       </c>
       <c r="J18">
+        <v>331</v>
+      </c>
+      <c r="K18">
         <v>486</v>
-      </c>
-      <c r="K18">
-        <f>I18/J18</f>
-        <v>0.68930041152263377</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>20340</v>
@@ -1313,7 +1308,7 @@
       <c r="E19">
         <v>30289</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="3">
         <v>25337</v>
       </c>
       <c r="H19">
@@ -1323,16 +1318,15 @@
         <v>32730</v>
       </c>
       <c r="J19">
+        <v>32747</v>
+      </c>
+      <c r="K19">
         <v>28443</v>
-      </c>
-      <c r="K19">
-        <f>I19/J19</f>
-        <v>1.1507224976268327</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>1370</v>
@@ -1346,7 +1340,7 @@
       <c r="E20">
         <v>2095</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>1753</v>
       </c>
       <c r="H20">
@@ -1354,11 +1348,14 @@
       </c>
       <c r="I20">
         <v>2264</v>
+      </c>
+      <c r="J20">
+        <v>2260</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>2206</v>
@@ -1372,7 +1369,7 @@
       <c r="E21">
         <v>2631</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="3">
         <v>2194</v>
       </c>
       <c r="H21">
@@ -1381,14 +1378,14 @@
       <c r="I21">
         <v>2611</v>
       </c>
+      <c r="J21">
+        <v>2619</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="25" ht="14.25">
-      <c r="B25"/>
-    </row>
+    <row r="25" ht="14.25"/>
     <row r="26" ht="14.25"/>
     <row r="27" ht="14.25"/>
     <row r="28" ht="14.25"/>
@@ -1415,6 +1412,246 @@
     <row r="49" ht="14.25"/>
   </sheetData>
   <conditionalFormatting sqref="C2:G2 I2">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:G3 I3">
+    <cfRule type="colorScale" priority="80">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:G4 I4">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:G5 I5">
+    <cfRule type="colorScale" priority="78">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:G6 I6">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:G7 I7">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:G8 I8">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:G9 I9">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:G10 I10">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:G11 I11">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:G12 I12">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:G13 I13">
+    <cfRule type="colorScale" priority="70">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:G14 I14">
+    <cfRule type="colorScale" priority="69">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:G15 I15">
+    <cfRule type="colorScale" priority="68">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:G16 I16">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:G17 I17">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:G18 I18">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:G19 I19">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:G20 I20">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:G21 I21">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:H2">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -1426,7 +1663,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:G3 I3">
+  <conditionalFormatting sqref="C3:H3">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -1438,7 +1675,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:G4 I4">
+  <conditionalFormatting sqref="C4:H4">
     <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
@@ -1450,7 +1687,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:G5 I5">
+  <conditionalFormatting sqref="C5:H5">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -1462,7 +1699,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:G6 I6">
+  <conditionalFormatting sqref="C6:H6">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -1474,7 +1711,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:G7 I7">
+  <conditionalFormatting sqref="C7:H7">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="min"/>
@@ -1486,7 +1723,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:G8 I8">
+  <conditionalFormatting sqref="C8:H8">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -1498,7 +1735,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:G9 I9">
+  <conditionalFormatting sqref="C9:H9">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
@@ -1510,7 +1747,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:G10 I10">
+  <conditionalFormatting sqref="C10:H10">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -1522,19 +1759,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:G11 I11">
+  <conditionalFormatting sqref="C11:H11">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:G12 I12">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:H11">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -1546,7 +1783,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:G13 I13">
+  <conditionalFormatting sqref="C12:H12">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -1558,7 +1795,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:G14 I14">
+  <conditionalFormatting sqref="C13:H13">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -1570,7 +1807,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:G15 I15">
+  <conditionalFormatting sqref="C14:H14">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -1582,7 +1819,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:G16 I16">
+  <conditionalFormatting sqref="C15:H15">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -1594,7 +1831,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:G17 I17">
+  <conditionalFormatting sqref="C16:H16">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -1606,7 +1843,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:G18 I18">
+  <conditionalFormatting sqref="C17:H17">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -1618,7 +1855,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:G19 I19">
+  <conditionalFormatting sqref="C18:H18">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -1630,7 +1867,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:G20 I20">
+  <conditionalFormatting sqref="C19:H19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -1642,7 +1879,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:G21 I21">
+  <conditionalFormatting sqref="C20:H20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -1654,7 +1891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:H2">
+  <conditionalFormatting sqref="C21:H21">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -1666,7 +1903,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:H3">
+  <conditionalFormatting sqref="C2:I2">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -1678,7 +1915,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:H4">
+  <conditionalFormatting sqref="C3:I3">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -1690,7 +1927,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:H5">
+  <conditionalFormatting sqref="C4:I4">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -1702,7 +1939,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:H6">
+  <conditionalFormatting sqref="C5:I5">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -1714,7 +1951,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:H7">
+  <conditionalFormatting sqref="C6:I6">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -1726,7 +1963,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:H8">
+  <conditionalFormatting sqref="C7:I7">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -1738,7 +1975,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:H9">
+  <conditionalFormatting sqref="C8:I8">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -1750,7 +1987,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:H10">
+  <conditionalFormatting sqref="C9:I9">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -1762,19 +1999,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:H11">
+  <conditionalFormatting sqref="C10:I10">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:H11">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:I11">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -1786,7 +2023,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:H12">
+  <conditionalFormatting sqref="C12:I12">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -1798,7 +2035,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:H13">
+  <conditionalFormatting sqref="C13:I13">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -1810,7 +2047,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:H14">
+  <conditionalFormatting sqref="C14:I14">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -1822,7 +2059,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:H15">
+  <conditionalFormatting sqref="C15:I15">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -1834,7 +2071,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:H16">
+  <conditionalFormatting sqref="C16:I16">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -1846,7 +2083,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:H17">
+  <conditionalFormatting sqref="C17:I17">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -1858,7 +2095,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:H18">
+  <conditionalFormatting sqref="C18:I18">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -1870,7 +2107,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:H19">
+  <conditionalFormatting sqref="C19:I19">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -1882,7 +2119,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:H20">
+  <conditionalFormatting sqref="C20:I20">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -1894,7 +2131,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:H21">
+  <conditionalFormatting sqref="C21:I21">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -1906,7 +2143,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I2">
+  <conditionalFormatting sqref="C2:J2">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -1918,7 +2155,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:I3">
+  <conditionalFormatting sqref="C3:J3">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1930,7 +2167,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:I4">
+  <conditionalFormatting sqref="C4:J4">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -1942,7 +2179,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I5">
+  <conditionalFormatting sqref="C5:J5">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -1954,7 +2191,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:I6">
+  <conditionalFormatting sqref="C6:J6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1966,7 +2203,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:I7">
+  <conditionalFormatting sqref="C7:J7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -1978,7 +2215,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:I8">
+  <conditionalFormatting sqref="C8:J8">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1990,7 +2227,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:I9">
+  <conditionalFormatting sqref="C9:J9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2002,7 +2239,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:I10">
+  <conditionalFormatting sqref="C10:J10">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -2014,7 +2251,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:I11">
+  <conditionalFormatting sqref="C11:J11">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -2026,7 +2263,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:I12">
+  <conditionalFormatting sqref="C12:J12">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2038,7 +2275,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:I13">
+  <conditionalFormatting sqref="C13:J13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2050,7 +2287,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:I14">
+  <conditionalFormatting sqref="C14:J14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2062,7 +2299,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:I15">
+  <conditionalFormatting sqref="C15:J15">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2074,7 +2311,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:I16">
+  <conditionalFormatting sqref="C16:J16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2086,7 +2323,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:I17">
+  <conditionalFormatting sqref="C17:J17">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2098,7 +2335,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:I18">
+  <conditionalFormatting sqref="C18:J18">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2110,7 +2347,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:I19">
+  <conditionalFormatting sqref="C19:J19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2122,7 +2359,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20:I20">
+  <conditionalFormatting sqref="C20:J20">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2134,7 +2371,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:I21">
+  <conditionalFormatting sqref="C21:J21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>